<commit_message>
Version 3.0 (BETA) Build 3025
Fixed :
[CR-015] Change wording in dictionary for ward Change request [CR]

[CR-014] Add Table S10A and S10B to display mapping of ward in Microbiology data and Hospital admission data files with dictionary for ward. Change request [CR]

[BUG-013] Annex A list of organism should be the same as version 2 (Full name) as well as Annex A1, A2 (Italic vs non-italic in the organism name) Bug
</commit_message>
<xml_diff>
--- a/AMASS3.0/Example_dataset_4_cluster_signals/dictionary_for_wards.xlsx
+++ b/AMASS3.0/Example_dataset_4_cluster_signals/dictionary_for_wards.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\AMASS3.0B3019\AMASS3.0-Lite-main\AMASS3.0\Example_Dataset_4_Cluster_Signal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ONGWORK\TEST\AMASS3.0B3024\AMASS3.0-Lite-main\AMASS3.0\Example_dataset_4_cluster_signals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C14B9B6-0EE0-47C6-9ABB-F8E5C82545F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36" yWindow="756" windowWidth="23004" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36" yWindow="756" windowWidth="23004" windowHeight="12204"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -39,9 +38,6 @@
     <t>Explanations</t>
   </si>
   <si>
-    <t>Ward name used in your microbiology_data</t>
-  </si>
-  <si>
     <t>ward_001</t>
   </si>
   <si>
@@ -498,9 +494,6 @@
     <t>Variable names used in AMASS</t>
   </si>
   <si>
-    <t>Variable names used in your microbiology data file</t>
-  </si>
-  <si>
     <t>Explanations - Variable names used in AMASS</t>
   </si>
   <si>
@@ -694,12 +687,18 @@
   </si>
   <si>
     <t>Group 5 (OTHERS)</t>
+  </si>
+  <si>
+    <t>Ward name used in your data files</t>
+  </si>
+  <si>
+    <t>Variable names used in your data files</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1165,7 +1164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="250" workbookViewId="0">
@@ -1184,10 +1183,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>154</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="6" t="s">
@@ -1199,37 +1198,37 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>156</v>
+        <v>221</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B4"/>
       <c r="C4" s="15"/>
@@ -1237,18 +1236,18 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>1</v>
@@ -1259,2416 +1258,2416 @@
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="D10" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="17"/>
       <c r="D11" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="17"/>
       <c r="D12" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="17"/>
       <c r="D13" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="17"/>
       <c r="D14" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="17"/>
       <c r="D15" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="17"/>
       <c r="D16" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="17"/>
       <c r="D17" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="17"/>
       <c r="D18" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="17"/>
       <c r="D19" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="17"/>
       <c r="D20" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="17"/>
       <c r="D21" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="17"/>
       <c r="D22" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="17"/>
       <c r="D23" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="17"/>
       <c r="D24" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="17"/>
       <c r="D25" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="17"/>
       <c r="D26" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="17"/>
       <c r="D27" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="17"/>
       <c r="D28" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="17"/>
       <c r="D29" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="17"/>
       <c r="D30" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="17"/>
       <c r="D31" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="17"/>
       <c r="D32" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="17"/>
       <c r="D33" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="17"/>
       <c r="D34" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="17"/>
       <c r="D35" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="17"/>
       <c r="D36" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="17"/>
       <c r="D37" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="17"/>
       <c r="D38" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="17"/>
       <c r="D39" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="17"/>
       <c r="D40" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="17"/>
       <c r="D41" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="17"/>
       <c r="D42" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="17"/>
       <c r="D43" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="17"/>
       <c r="D44" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="17"/>
       <c r="D45" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="17"/>
       <c r="D46" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="17"/>
       <c r="D47" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="17"/>
       <c r="D48" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="17"/>
       <c r="D49" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="17"/>
       <c r="D50" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="17"/>
       <c r="D51" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="17"/>
       <c r="D52" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="17"/>
       <c r="D53" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="17"/>
       <c r="D54" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="17"/>
       <c r="D55" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="17"/>
       <c r="D56" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="17"/>
       <c r="D57" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="17"/>
       <c r="D58" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="17"/>
       <c r="D59" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="17"/>
       <c r="D60" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="17"/>
       <c r="D61" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="17"/>
       <c r="D62" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="17"/>
       <c r="D63" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="17"/>
       <c r="D64" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="17"/>
       <c r="D65" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="17"/>
       <c r="D66" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="17"/>
       <c r="D67" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="17"/>
       <c r="D68" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" s="17"/>
       <c r="D69" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="17"/>
       <c r="D70" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="17"/>
       <c r="D71" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="17"/>
       <c r="D72" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="17"/>
       <c r="D73" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="17"/>
       <c r="D74" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="17"/>
       <c r="D75" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" s="17"/>
       <c r="D76" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" s="17"/>
       <c r="D77" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" s="17"/>
       <c r="D78" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" s="17"/>
       <c r="D79" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="17"/>
       <c r="D80" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="17"/>
       <c r="D81" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="17"/>
       <c r="D82" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="17"/>
       <c r="D83" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="17"/>
       <c r="D84" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" s="17"/>
       <c r="D85" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" s="17"/>
       <c r="D86" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" s="17"/>
       <c r="D87" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" s="17"/>
       <c r="D88" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" s="17"/>
       <c r="D89" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" s="17"/>
       <c r="D90" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" s="17"/>
       <c r="D91" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" s="17"/>
       <c r="D92" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" s="17"/>
       <c r="D93" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" s="17"/>
       <c r="D94" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" s="17"/>
       <c r="D95" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" s="17"/>
       <c r="D96" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" s="17"/>
       <c r="D97" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" s="17"/>
       <c r="D98" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" s="17"/>
       <c r="D99" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" s="17"/>
       <c r="D100" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" s="17"/>
       <c r="D101" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" s="17"/>
       <c r="D102" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" s="17"/>
       <c r="D103" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" s="17"/>
       <c r="D104" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" s="17"/>
       <c r="D105" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" s="17"/>
       <c r="D106" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107" s="17"/>
       <c r="D107" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108" s="17"/>
       <c r="D108" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" s="17"/>
       <c r="D109" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" s="17"/>
       <c r="D110" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" s="17"/>
       <c r="D111" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" s="17"/>
       <c r="D112" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113" s="17"/>
       <c r="D113" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" s="17"/>
       <c r="D114" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" s="17"/>
       <c r="D115" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" s="17"/>
       <c r="D116" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117" s="17"/>
       <c r="D117" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118" s="17"/>
       <c r="D118" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" s="17"/>
       <c r="D119" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" s="17"/>
       <c r="D120" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" s="17"/>
       <c r="D121" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" s="17"/>
       <c r="D122" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" s="17"/>
       <c r="D123" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124" s="17"/>
       <c r="D124" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125" s="17"/>
       <c r="D125" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126" s="17"/>
       <c r="D126" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B127" s="17"/>
       <c r="D127" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128" s="17"/>
       <c r="D128" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129" s="17"/>
       <c r="D129" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130" s="17"/>
       <c r="D130" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" s="17"/>
       <c r="D131" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132" s="17"/>
       <c r="D132" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" s="17"/>
       <c r="D133" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" s="17"/>
       <c r="D134" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" s="17"/>
       <c r="D135" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136" s="17"/>
       <c r="D136" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137" s="17"/>
       <c r="D137" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138" s="17"/>
       <c r="D138" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139" s="17"/>
       <c r="D139" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140" s="17"/>
       <c r="D140" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" s="17"/>
       <c r="D141" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B142" s="17"/>
       <c r="D142" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B143" s="17"/>
       <c r="D143" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B144" s="17"/>
       <c r="D144" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B145" s="17"/>
       <c r="D145" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B146" s="17"/>
       <c r="D146" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B147" s="17"/>
       <c r="D147" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B148" s="17"/>
       <c r="D148" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B149" s="17"/>
       <c r="D149" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B150" s="17"/>
       <c r="D150" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B151" s="17"/>
       <c r="D151" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B152" s="17"/>
       <c r="D152" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B153" s="17"/>
       <c r="D153" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B154" s="17"/>
       <c r="D154" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B155" s="17"/>
       <c r="D155" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B156" s="17"/>
       <c r="D156" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B157" s="17"/>
       <c r="D157" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B158" s="17"/>
       <c r="D158" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B159" s="17"/>
       <c r="D159" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B160" s="17"/>
       <c r="D160" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B161" s="17"/>
       <c r="D161" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B162" s="17"/>
       <c r="D162" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B163" s="17"/>
       <c r="D163" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B164" s="17"/>
       <c r="D164" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B165" s="17"/>
       <c r="D165" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B166" s="17"/>
       <c r="D166" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B167" s="17"/>
       <c r="D167" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B168" s="17"/>
       <c r="D168" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B169" s="17"/>
       <c r="D169" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B170" s="17"/>
       <c r="D170" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B171" s="17"/>
       <c r="D171" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B172" s="17"/>
       <c r="D172" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B173" s="17"/>
       <c r="D173" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B174" s="17"/>
       <c r="D174" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B175" s="17"/>
       <c r="D175" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B176" s="17"/>
       <c r="D176" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B177" s="17"/>
       <c r="D177" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B178" s="17"/>
       <c r="D178" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B179" s="17"/>
       <c r="D179" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B180" s="17"/>
       <c r="D180" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B181" s="17"/>
       <c r="D181" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B182" s="17"/>
       <c r="D182" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B183" s="17"/>
       <c r="D183" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B184" s="17"/>
       <c r="D184" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B185" s="17"/>
       <c r="D185" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D186" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D187" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D188" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D189" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D190" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D191" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D192" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D193" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E193" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D194" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D195" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E195" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D196" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E196" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D197" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E197" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D198" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E198" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D199" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E199" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D200" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D201" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E201" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D202" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E202" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D203" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E203" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D204" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D205" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M19:M48">
+  <sortState ref="M19:M48">
     <sortCondition ref="M18:M48"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ward type is invalid" error="Please select a ward type from the dropdown list provided. Otherwise, this ward type will not be included for the analysis." sqref="C6:C205" xr:uid="{C05A4E33-6BDE-464C-84BA-EEC0D69E7404}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ward type is invalid" error="Please select a ward type from the dropdown list provided. Otherwise, this ward type will not be included for the analysis." sqref="C6:C205">
       <formula1>"Group 1 (MED),Group 2 (PED),Group 3 (SURG),Group 4 (ORTHO),Group 5 (OTHERS)"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Version 3.0 Build 3029
Fix:
[Bug-026] AMR Surveillance report not generate Annex B
[Bug-027] Data_verification_logfile report Table S8 shows an incorrect table
[CR-017] Add Ofloxacin in example/template dictionary for microbiology data
[CR-020] Annex C move configs from the Annex C constant file to configuration file
</commit_message>
<xml_diff>
--- a/AMASS3.0/Example_dataset_4_cluster_signals/dictionary_for_wards.xlsx
+++ b/AMASS3.0/Example_dataset_4_cluster_signals/dictionary_for_wards.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ONGWORK\TEST\AMASS3.0B3024\AMASS3.0-Lite-main\AMASS3.0\Example_dataset_4_cluster_signals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AMASS3.0.29.1-Lite-main\AMASS3.0-Lite-main\AMASS3.0\Example_dataset_4_cluster_signals\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA360ABE-779A-488A-9925-DA161974786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36" yWindow="756" windowWidth="23004" windowHeight="12204"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="224">
   <si>
     <t>Optional</t>
   </si>
@@ -680,25 +681,31 @@
     <t>female medical ward</t>
   </si>
   <si>
-    <t>female medical ward 2</t>
-  </si>
-  <si>
     <t>department</t>
   </si>
   <si>
-    <t>Group 5 (OTHERS)</t>
-  </si>
-  <si>
     <t>Ward name used in your data files</t>
   </si>
   <si>
     <t>Variable names used in your data files</t>
+  </si>
+  <si>
+    <t>male medical ward 3</t>
+  </si>
+  <si>
+    <t>Group 1 (MED)</t>
+  </si>
+  <si>
+    <t>female surgery ward</t>
+  </si>
+  <si>
+    <t>Group 3 (SURG)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -798,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -844,6 +851,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1164,24 +1174,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="84" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="105.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="36.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>152</v>
       </c>
@@ -1196,12 +1206,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>154</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="9" t="s">
@@ -1211,12 +1221,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="5" t="s">
@@ -1226,7 +1236,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>212</v>
       </c>
@@ -1239,12 +1249,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>156</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>210</v>
@@ -1256,7 +1266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
@@ -1264,7 +1274,7 @@
         <v>213</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>0</v>
@@ -1273,7 +1283,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>4</v>
       </c>
@@ -1281,7 +1291,7 @@
         <v>214</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>0</v>
@@ -1290,7 +1300,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
@@ -1298,7 +1308,7 @@
         <v>215</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>0</v>
@@ -1307,7 +1317,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>6</v>
       </c>
@@ -1315,7 +1325,7 @@
         <v>216</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>0</v>
@@ -1324,15 +1334,15 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
-        <v>217</v>
+      <c r="B10" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>0</v>
@@ -1341,11 +1351,16 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="D11" s="14" t="s">
         <v>0</v>
       </c>
@@ -1353,7 +1368,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>9</v>
       </c>
@@ -1365,7 +1380,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>10</v>
       </c>
@@ -1377,7 +1392,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>11</v>
       </c>
@@ -1389,7 +1404,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>12</v>
       </c>
@@ -1401,7 +1416,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>13</v>
       </c>
@@ -1413,7 +1428,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>14</v>
       </c>
@@ -1425,7 +1440,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>15</v>
       </c>
@@ -1437,7 +1452,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>16</v>
       </c>
@@ -1449,7 +1464,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>17</v>
       </c>
@@ -1461,7 +1476,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -1473,7 +1488,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>19</v>
       </c>
@@ -1485,7 +1500,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>20</v>
       </c>
@@ -1497,7 +1512,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>21</v>
       </c>
@@ -1509,7 +1524,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>22</v>
       </c>
@@ -1521,7 +1536,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>23</v>
       </c>
@@ -1533,7 +1548,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>24</v>
       </c>
@@ -1545,7 +1560,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>25</v>
       </c>
@@ -1557,7 +1572,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>26</v>
       </c>
@@ -1569,7 +1584,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>27</v>
       </c>
@@ -1581,7 +1596,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>28</v>
       </c>
@@ -1593,7 +1608,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>29</v>
       </c>
@@ -1605,7 +1620,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>30</v>
       </c>
@@ -1617,7 +1632,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>31</v>
       </c>
@@ -1629,7 +1644,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>32</v>
       </c>
@@ -1641,7 +1656,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>33</v>
       </c>
@@ -1653,7 +1668,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
         <v>34</v>
       </c>
@@ -1665,7 +1680,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>35</v>
       </c>
@@ -1677,7 +1692,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
         <v>36</v>
       </c>
@@ -1689,7 +1704,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
         <v>37</v>
       </c>
@@ -1701,7 +1716,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
         <v>38</v>
       </c>
@@ -1713,7 +1728,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
         <v>39</v>
       </c>
@@ -1725,7 +1740,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
         <v>40</v>
       </c>
@@ -1737,7 +1752,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
         <v>41</v>
       </c>
@@ -1749,7 +1764,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
         <v>42</v>
       </c>
@@ -1761,7 +1776,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
         <v>43</v>
       </c>
@@ -1773,7 +1788,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
         <v>44</v>
       </c>
@@ -1785,7 +1800,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
         <v>45</v>
       </c>
@@ -1797,7 +1812,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
         <v>46</v>
       </c>
@@ -1809,7 +1824,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
         <v>47</v>
       </c>
@@ -1821,7 +1836,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
         <v>48</v>
       </c>
@@ -1833,7 +1848,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
         <v>49</v>
       </c>
@@ -1845,7 +1860,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
         <v>50</v>
       </c>
@@ -1857,7 +1872,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
         <v>51</v>
       </c>
@@ -1869,7 +1884,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
         <v>52</v>
       </c>
@@ -1881,7 +1896,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="13" t="s">
         <v>53</v>
       </c>
@@ -1893,7 +1908,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
         <v>54</v>
       </c>
@@ -1905,7 +1920,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
         <v>55</v>
       </c>
@@ -1917,7 +1932,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
         <v>56</v>
       </c>
@@ -1929,7 +1944,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="13" t="s">
         <v>57</v>
       </c>
@@ -1941,7 +1956,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
         <v>58</v>
       </c>
@@ -1953,7 +1968,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="13" t="s">
         <v>59</v>
       </c>
@@ -1965,7 +1980,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
         <v>60</v>
       </c>
@@ -1977,7 +1992,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
         <v>61</v>
       </c>
@@ -1989,7 +2004,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="13" t="s">
         <v>62</v>
       </c>
@@ -2001,7 +2016,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="13" t="s">
         <v>63</v>
       </c>
@@ -2013,7 +2028,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
         <v>64</v>
       </c>
@@ -2025,7 +2040,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
         <v>65</v>
       </c>
@@ -2037,7 +2052,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="13" t="s">
         <v>66</v>
       </c>
@@ -2049,7 +2064,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="13" t="s">
         <v>67</v>
       </c>
@@ -2061,7 +2076,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="13" t="s">
         <v>68</v>
       </c>
@@ -2073,7 +2088,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="13" t="s">
         <v>69</v>
       </c>
@@ -2085,7 +2100,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="13" t="s">
         <v>70</v>
       </c>
@@ -2097,7 +2112,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
         <v>71</v>
       </c>
@@ -2109,7 +2124,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="13" t="s">
         <v>72</v>
       </c>
@@ -2121,7 +2136,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="13" t="s">
         <v>73</v>
       </c>
@@ -2133,7 +2148,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="13" t="s">
         <v>74</v>
       </c>
@@ -2145,7 +2160,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
         <v>75</v>
       </c>
@@ -2157,7 +2172,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>76</v>
       </c>
@@ -2169,7 +2184,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="13" t="s">
         <v>77</v>
       </c>
@@ -2181,7 +2196,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="13" t="s">
         <v>78</v>
       </c>
@@ -2193,7 +2208,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="13" t="s">
         <v>79</v>
       </c>
@@ -2205,7 +2220,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="13" t="s">
         <v>80</v>
       </c>
@@ -2217,7 +2232,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="13" t="s">
         <v>81</v>
       </c>
@@ -2229,7 +2244,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="13" t="s">
         <v>82</v>
       </c>
@@ -2241,7 +2256,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="13" t="s">
         <v>83</v>
       </c>
@@ -2253,7 +2268,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="13" t="s">
         <v>84</v>
       </c>
@@ -2265,7 +2280,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="13" t="s">
         <v>85</v>
       </c>
@@ -2277,7 +2292,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="13" t="s">
         <v>86</v>
       </c>
@@ -2289,7 +2304,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="13" t="s">
         <v>87</v>
       </c>
@@ -2301,7 +2316,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="13" t="s">
         <v>88</v>
       </c>
@@ -2313,7 +2328,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="13" t="s">
         <v>89</v>
       </c>
@@ -2325,7 +2340,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="13" t="s">
         <v>90</v>
       </c>
@@ -2337,7 +2352,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="13" t="s">
         <v>91</v>
       </c>
@@ -2349,7 +2364,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="13" t="s">
         <v>92</v>
       </c>
@@ -2361,7 +2376,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="13" t="s">
         <v>93</v>
       </c>
@@ -2373,7 +2388,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="13" t="s">
         <v>94</v>
       </c>
@@ -2385,7 +2400,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="13" t="s">
         <v>95</v>
       </c>
@@ -2397,7 +2412,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="13" t="s">
         <v>96</v>
       </c>
@@ -2409,7 +2424,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="13" t="s">
         <v>97</v>
       </c>
@@ -2421,7 +2436,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="13" t="s">
         <v>98</v>
       </c>
@@ -2433,7 +2448,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="13" t="s">
         <v>99</v>
       </c>
@@ -2445,7 +2460,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="13" t="s">
         <v>100</v>
       </c>
@@ -2457,7 +2472,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="13" t="s">
         <v>101</v>
       </c>
@@ -2469,7 +2484,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="13" t="s">
         <v>102</v>
       </c>
@@ -2481,7 +2496,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="13" t="s">
         <v>103</v>
       </c>
@@ -2493,7 +2508,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="13" t="s">
         <v>104</v>
       </c>
@@ -2505,7 +2520,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="13" t="s">
         <v>105</v>
       </c>
@@ -2517,7 +2532,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="13" t="s">
         <v>106</v>
       </c>
@@ -2529,7 +2544,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="13" t="s">
         <v>107</v>
       </c>
@@ -2541,7 +2556,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="13" t="s">
         <v>108</v>
       </c>
@@ -2553,7 +2568,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="13" t="s">
         <v>109</v>
       </c>
@@ -2565,7 +2580,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="13" t="s">
         <v>110</v>
       </c>
@@ -2577,7 +2592,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="13" t="s">
         <v>111</v>
       </c>
@@ -2589,7 +2604,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="13" t="s">
         <v>112</v>
       </c>
@@ -2601,7 +2616,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="13" t="s">
         <v>113</v>
       </c>
@@ -2613,7 +2628,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="13" t="s">
         <v>114</v>
       </c>
@@ -2625,7 +2640,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="13" t="s">
         <v>115</v>
       </c>
@@ -2637,7 +2652,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="13" t="s">
         <v>116</v>
       </c>
@@ -2649,7 +2664,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="13" t="s">
         <v>117</v>
       </c>
@@ -2661,7 +2676,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="13" t="s">
         <v>118</v>
       </c>
@@ -2673,7 +2688,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="13" t="s">
         <v>119</v>
       </c>
@@ -2685,7 +2700,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="13" t="s">
         <v>120</v>
       </c>
@@ -2697,7 +2712,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="13" t="s">
         <v>121</v>
       </c>
@@ -2709,7 +2724,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="13" t="s">
         <v>122</v>
       </c>
@@ -2721,7 +2736,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="13" t="s">
         <v>123</v>
       </c>
@@ -2733,7 +2748,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="13" t="s">
         <v>124</v>
       </c>
@@ -2745,7 +2760,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="13" t="s">
         <v>125</v>
       </c>
@@ -2757,7 +2772,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="13" t="s">
         <v>126</v>
       </c>
@@ -2769,7 +2784,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="13" t="s">
         <v>127</v>
       </c>
@@ -2781,7 +2796,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="13" t="s">
         <v>128</v>
       </c>
@@ -2793,7 +2808,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="13" t="s">
         <v>129</v>
       </c>
@@ -2805,7 +2820,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="13" t="s">
         <v>130</v>
       </c>
@@ -2817,7 +2832,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="13" t="s">
         <v>131</v>
       </c>
@@ -2829,7 +2844,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="13" t="s">
         <v>132</v>
       </c>
@@ -2841,7 +2856,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="13" t="s">
         <v>133</v>
       </c>
@@ -2853,7 +2868,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="13" t="s">
         <v>134</v>
       </c>
@@ -2865,7 +2880,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="13" t="s">
         <v>135</v>
       </c>
@@ -2877,7 +2892,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="13" t="s">
         <v>136</v>
       </c>
@@ -2889,7 +2904,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="13" t="s">
         <v>137</v>
       </c>
@@ -2901,7 +2916,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="13" t="s">
         <v>138</v>
       </c>
@@ -2913,7 +2928,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="13" t="s">
         <v>139</v>
       </c>
@@ -2925,7 +2940,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="13" t="s">
         <v>140</v>
       </c>
@@ -2937,7 +2952,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="13" t="s">
         <v>141</v>
       </c>
@@ -2949,7 +2964,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="13" t="s">
         <v>142</v>
       </c>
@@ -2961,7 +2976,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="13" t="s">
         <v>143</v>
       </c>
@@ -2973,7 +2988,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="13" t="s">
         <v>144</v>
       </c>
@@ -2985,7 +3000,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="13" t="s">
         <v>145</v>
       </c>
@@ -2997,7 +3012,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="13" t="s">
         <v>146</v>
       </c>
@@ -3009,7 +3024,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="13" t="s">
         <v>147</v>
       </c>
@@ -3021,7 +3036,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="13" t="s">
         <v>148</v>
       </c>
@@ -3033,7 +3048,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="13" t="s">
         <v>149</v>
       </c>
@@ -3045,7 +3060,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="13" t="s">
         <v>157</v>
       </c>
@@ -3057,7 +3072,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="13" t="s">
         <v>158</v>
       </c>
@@ -3069,7 +3084,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="13" t="s">
         <v>159</v>
       </c>
@@ -3081,7 +3096,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="13" t="s">
         <v>160</v>
       </c>
@@ -3093,7 +3108,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="13" t="s">
         <v>161</v>
       </c>
@@ -3105,7 +3120,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="13" t="s">
         <v>162</v>
       </c>
@@ -3117,7 +3132,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="13" t="s">
         <v>163</v>
       </c>
@@ -3129,7 +3144,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="13" t="s">
         <v>164</v>
       </c>
@@ -3141,7 +3156,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="13" t="s">
         <v>165</v>
       </c>
@@ -3153,7 +3168,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="13" t="s">
         <v>166</v>
       </c>
@@ -3165,7 +3180,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="13" t="s">
         <v>167</v>
       </c>
@@ -3177,7 +3192,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="13" t="s">
         <v>168</v>
       </c>
@@ -3189,7 +3204,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="13" t="s">
         <v>169</v>
       </c>
@@ -3201,7 +3216,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="13" t="s">
         <v>170</v>
       </c>
@@ -3213,7 +3228,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="13" t="s">
         <v>171</v>
       </c>
@@ -3225,7 +3240,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="13" t="s">
         <v>172</v>
       </c>
@@ -3237,7 +3252,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="13" t="s">
         <v>173</v>
       </c>
@@ -3249,7 +3264,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="13" t="s">
         <v>174</v>
       </c>
@@ -3261,7 +3276,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="13" t="s">
         <v>175</v>
       </c>
@@ -3273,7 +3288,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="13" t="s">
         <v>176</v>
       </c>
@@ -3285,7 +3300,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="13" t="s">
         <v>177</v>
       </c>
@@ -3297,7 +3312,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="13" t="s">
         <v>178</v>
       </c>
@@ -3309,7 +3324,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="13" t="s">
         <v>179</v>
       </c>
@@ -3321,7 +3336,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="13" t="s">
         <v>180</v>
       </c>
@@ -3333,7 +3348,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="13" t="s">
         <v>181</v>
       </c>
@@ -3345,7 +3360,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="13" t="s">
         <v>182</v>
       </c>
@@ -3357,7 +3372,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="13" t="s">
         <v>183</v>
       </c>
@@ -3369,7 +3384,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="13" t="s">
         <v>184</v>
       </c>
@@ -3381,7 +3396,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="13" t="s">
         <v>185</v>
       </c>
@@ -3393,7 +3408,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="13" t="s">
         <v>186</v>
       </c>
@@ -3405,7 +3420,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="13" t="s">
         <v>187</v>
       </c>
@@ -3417,7 +3432,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="13" t="s">
         <v>188</v>
       </c>
@@ -3429,7 +3444,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="13" t="s">
         <v>189</v>
       </c>
@@ -3441,7 +3456,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="13" t="s">
         <v>190</v>
       </c>
@@ -3452,7 +3467,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="13" t="s">
         <v>191</v>
       </c>
@@ -3463,7 +3478,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="13" t="s">
         <v>192</v>
       </c>
@@ -3474,7 +3489,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="13" t="s">
         <v>193</v>
       </c>
@@ -3485,7 +3500,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="13" t="s">
         <v>194</v>
       </c>
@@ -3496,7 +3511,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="13" t="s">
         <v>195</v>
       </c>
@@ -3507,7 +3522,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="13" t="s">
         <v>196</v>
       </c>
@@ -3518,7 +3533,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="13" t="s">
         <v>197</v>
       </c>
@@ -3529,7 +3544,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="13" t="s">
         <v>198</v>
       </c>
@@ -3540,7 +3555,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="13" t="s">
         <v>199</v>
       </c>
@@ -3551,7 +3566,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="13" t="s">
         <v>200</v>
       </c>
@@ -3562,7 +3577,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="13" t="s">
         <v>201</v>
       </c>
@@ -3573,7 +3588,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="13" t="s">
         <v>202</v>
       </c>
@@ -3584,7 +3599,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="13" t="s">
         <v>203</v>
       </c>
@@ -3595,7 +3610,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="13" t="s">
         <v>204</v>
       </c>
@@ -3606,7 +3621,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="13" t="s">
         <v>205</v>
       </c>
@@ -3617,7 +3632,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="13" t="s">
         <v>206</v>
       </c>
@@ -3628,7 +3643,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="13" t="s">
         <v>207</v>
       </c>
@@ -3639,7 +3654,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="13" t="s">
         <v>208</v>
       </c>
@@ -3650,7 +3665,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="13" t="s">
         <v>209</v>
       </c>
@@ -3662,12 +3677,12 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="M19:M48">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M19:M48">
     <sortCondition ref="M18:M48"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ward type is invalid" error="Please select a ward type from the dropdown list provided. Otherwise, this ward type will not be included for the analysis." sqref="C6:C205">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ward type is invalid" error="Please select a ward type from the dropdown list provided. Otherwise, this ward type will not be included for the analysis." sqref="C6:C205" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Group 1 (MED),Group 2 (PED),Group 3 (SURG),Group 4 (ORTHO),Group 5 (OTHERS)"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>